<commit_message>
Finished analysis and graphic generation
</commit_message>
<xml_diff>
--- a/FinalProject/DataSets/Team_Year_Rankings.xlsx
+++ b/FinalProject/DataSets/Team_Year_Rankings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\MSU\Junior\Spring 2020\SSC442\Final Project\Data Sets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\MSU\Junior\Spring 2020\SSC442\Final Project\SSC442Team7\FinalProject\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20954676-ACBC-48AF-B946-BB5618C85260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B4376C-58F9-4FD9-90A0-03D0EF734598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C08542D5-3DD7-46A2-BC0F-684C4B996726}"/>
   </bookViews>
@@ -128,75 +128,6 @@
     <t>Team</t>
   </si>
   <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>PA</t>
-  </si>
-  <si>
-    <t>WI</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>NV</t>
-  </si>
-  <si>
-    <t>MN</t>
-  </si>
-  <si>
-    <t>MO</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>IL</t>
-  </si>
-  <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>MI</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>AZ</t>
-  </si>
-  <si>
-    <t>NC</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
     <t>Cardinals</t>
   </si>
   <si>
@@ -309,6 +240,75 @@
   </si>
   <si>
     <t>WonSuperBowl</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>NorthCarolina</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Massachusets</t>
+  </si>
+  <si>
+    <t>WashingtonD. C.</t>
   </si>
 </sst>
 </file>
@@ -663,13 +663,13 @@
   <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J92" sqref="J92"/>
+      <selection activeCell="K10" sqref="K10:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
@@ -686,16 +686,16 @@
         <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -703,10 +703,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D2">
         <v>2018</v>
@@ -726,10 +726,10 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>2018</v>
@@ -749,10 +749,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>2018</v>
@@ -772,10 +772,10 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D5">
         <v>2018</v>
@@ -795,10 +795,10 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>2018</v>
@@ -818,10 +818,10 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>2018</v>
@@ -841,10 +841,10 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D8">
         <v>2018</v>
@@ -864,10 +864,10 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <v>2018</v>
@@ -887,10 +887,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D10">
         <v>2018</v>
@@ -910,10 +910,10 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>2018</v>
@@ -933,10 +933,10 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>2018</v>
@@ -956,10 +956,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D13">
         <v>2018</v>
@@ -979,10 +979,10 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D14">
         <v>2018</v>
@@ -1002,10 +1002,10 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>2018</v>
@@ -1022,13 +1022,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>2018</v>
@@ -1048,10 +1048,10 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D17">
         <v>2018</v>
@@ -1071,10 +1071,10 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D18">
         <v>2018</v>
@@ -1094,10 +1094,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>2018</v>
@@ -1117,10 +1117,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D20">
         <v>2018</v>
@@ -1140,10 +1140,10 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <v>2018</v>
@@ -1163,10 +1163,10 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D22">
         <v>2018</v>
@@ -1186,10 +1186,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="D23">
         <v>2018</v>
@@ -1209,10 +1209,10 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D24">
         <v>2018</v>
@@ -1232,10 +1232,10 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D25">
         <v>2018</v>
@@ -1255,10 +1255,10 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D26">
         <v>2018</v>
@@ -1278,10 +1278,10 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D27">
         <v>2018</v>
@@ -1301,10 +1301,10 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D28">
         <v>2018</v>
@@ -1324,10 +1324,10 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="D29">
         <v>2018</v>
@@ -1347,10 +1347,10 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D30">
         <v>2018</v>
@@ -1370,10 +1370,10 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="D31">
         <v>2018</v>
@@ -1390,13 +1390,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D32">
         <v>2018</v>
@@ -1416,10 +1416,10 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D33">
         <v>2018</v>
@@ -1439,10 +1439,10 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D34">
         <v>2017</v>
@@ -1462,10 +1462,10 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D35">
         <v>2017</v>
@@ -1485,10 +1485,10 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="D36">
         <v>2017</v>
@@ -1508,10 +1508,10 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D37">
         <v>2017</v>
@@ -1531,10 +1531,10 @@
         <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D38">
         <v>2017</v>
@@ -1554,10 +1554,10 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D39">
         <v>2017</v>
@@ -1577,10 +1577,10 @@
         <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D40">
         <v>2017</v>
@@ -1600,10 +1600,10 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D41">
         <v>2017</v>
@@ -1623,10 +1623,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D42">
         <v>2017</v>
@@ -1646,10 +1646,10 @@
         <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D43">
         <v>2017</v>
@@ -1669,10 +1669,10 @@
         <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D44">
         <v>2017</v>
@@ -1692,10 +1692,10 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D45">
         <v>2017</v>
@@ -1715,10 +1715,10 @@
         <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D46">
         <v>2017</v>
@@ -1738,10 +1738,10 @@
         <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D47">
         <v>2017</v>
@@ -1758,13 +1758,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D48">
         <v>2017</v>
@@ -1784,10 +1784,10 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D49">
         <v>2017</v>
@@ -1807,10 +1807,10 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D50">
         <v>2017</v>
@@ -1830,10 +1830,10 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D51">
         <v>2017</v>
@@ -1853,10 +1853,10 @@
         <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C52" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D52">
         <v>2017</v>
@@ -1876,10 +1876,10 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D53">
         <v>2017</v>
@@ -1899,10 +1899,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D54">
         <v>2017</v>
@@ -1922,10 +1922,10 @@
         <v>23</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="D55">
         <v>2017</v>
@@ -1945,10 +1945,10 @@
         <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D56">
         <v>2017</v>
@@ -1968,10 +1968,10 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C57" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D57">
         <v>2017</v>
@@ -1991,10 +1991,10 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D58">
         <v>2017</v>
@@ -2014,10 +2014,10 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D59">
         <v>2017</v>
@@ -2037,10 +2037,10 @@
         <v>25</v>
       </c>
       <c r="B60" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C60" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D60">
         <v>2017</v>
@@ -2060,10 +2060,10 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C61" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="D61">
         <v>2017</v>
@@ -2083,10 +2083,10 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D62">
         <v>2017</v>
@@ -2106,10 +2106,10 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="C63" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="D63">
         <v>2017</v>
@@ -2126,13 +2126,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D64">
         <v>2017</v>
@@ -2152,10 +2152,10 @@
         <v>20</v>
       </c>
       <c r="B65" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D65">
         <v>2017</v>
@@ -2175,10 +2175,10 @@
         <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D66">
         <v>2016</v>
@@ -2198,10 +2198,10 @@
         <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C67" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D67">
         <v>2016</v>
@@ -2221,10 +2221,10 @@
         <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="D68">
         <v>2016</v>
@@ -2244,10 +2244,10 @@
         <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C69" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D69">
         <v>2016</v>
@@ -2267,10 +2267,10 @@
         <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D70">
         <v>2016</v>
@@ -2290,10 +2290,10 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D71">
         <v>2016</v>
@@ -2313,10 +2313,10 @@
         <v>28</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D72">
         <v>2016</v>
@@ -2336,10 +2336,10 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C73" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D73">
         <v>2016</v>
@@ -2359,10 +2359,10 @@
         <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C74" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D74">
         <v>2016</v>
@@ -2382,10 +2382,10 @@
         <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D75">
         <v>2016</v>
@@ -2405,10 +2405,10 @@
         <v>22</v>
       </c>
       <c r="B76" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D76">
         <v>2016</v>
@@ -2428,10 +2428,10 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="C77" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D77">
         <v>2016</v>
@@ -2451,10 +2451,10 @@
         <v>24</v>
       </c>
       <c r="B78" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C78" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D78">
         <v>2016</v>
@@ -2474,10 +2474,10 @@
         <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C79" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D79">
         <v>2016</v>
@@ -2494,13 +2494,13 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C80" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D80">
         <v>2016</v>
@@ -2520,10 +2520,10 @@
         <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D81">
         <v>2016</v>
@@ -2543,10 +2543,10 @@
         <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="C82" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D82">
         <v>2016</v>
@@ -2566,10 +2566,10 @@
         <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C83" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D83">
         <v>2016</v>
@@ -2589,10 +2589,10 @@
         <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C84" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D84">
         <v>2016</v>
@@ -2612,10 +2612,10 @@
         <v>13</v>
       </c>
       <c r="B85" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C85" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D85">
         <v>2016</v>
@@ -2635,10 +2635,10 @@
         <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="C86" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D86">
         <v>2016</v>
@@ -2658,10 +2658,10 @@
         <v>23</v>
       </c>
       <c r="B87" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C87" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="D87">
         <v>2016</v>
@@ -2681,10 +2681,10 @@
         <v>18</v>
       </c>
       <c r="B88" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C88" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D88">
         <v>2016</v>
@@ -2704,10 +2704,10 @@
         <v>10</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C89" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D89">
         <v>2016</v>
@@ -2727,10 +2727,10 @@
         <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C90" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D90">
         <v>2016</v>
@@ -2750,10 +2750,10 @@
         <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C91" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D91">
         <v>2016</v>
@@ -2773,10 +2773,10 @@
         <v>25</v>
       </c>
       <c r="B92" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C92" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D92">
         <v>2016</v>
@@ -2796,10 +2796,10 @@
         <v>12</v>
       </c>
       <c r="B93" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C93" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="D93">
         <v>2016</v>
@@ -2819,10 +2819,10 @@
         <v>5</v>
       </c>
       <c r="B94" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C94" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D94">
         <v>2016</v>
@@ -2842,10 +2842,10 @@
         <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="C95" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="D95">
         <v>2016</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B96" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C96" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D96">
         <v>2016</v>
@@ -2888,10 +2888,10 @@
         <v>20</v>
       </c>
       <c r="B97" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="C97" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D97">
         <v>2016</v>
@@ -2911,10 +2911,10 @@
         <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="C98" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D98">
         <v>2015</v>
@@ -2934,10 +2934,10 @@
         <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C99" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D99">
         <v>2015</v>
@@ -2957,10 +2957,10 @@
         <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C100" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="D100">
         <v>2015</v>
@@ -2980,10 +2980,10 @@
         <v>21</v>
       </c>
       <c r="B101" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C101" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D101">
         <v>2015</v>
@@ -3003,10 +3003,10 @@
         <v>26</v>
       </c>
       <c r="B102" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C102" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D102">
         <v>2015</v>
@@ -3026,10 +3026,10 @@
         <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C103" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D103">
         <v>2015</v>
@@ -3049,10 +3049,10 @@
         <v>28</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C104" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D104">
         <v>2015</v>
@@ -3072,10 +3072,10 @@
         <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C105" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D105">
         <v>2015</v>
@@ -3095,10 +3095,10 @@
         <v>1</v>
       </c>
       <c r="B106" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C106" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D106">
         <v>2015</v>
@@ -3118,10 +3118,10 @@
         <v>14</v>
       </c>
       <c r="B107" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C107" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D107">
         <v>2015</v>
@@ -3141,10 +3141,10 @@
         <v>22</v>
       </c>
       <c r="B108" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C108" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D108">
         <v>2015</v>
@@ -3164,10 +3164,10 @@
         <v>4</v>
       </c>
       <c r="B109" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="C109" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D109">
         <v>2015</v>
@@ -3187,10 +3187,10 @@
         <v>24</v>
       </c>
       <c r="B110" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C110" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D110">
         <v>2015</v>
@@ -3210,10 +3210,10 @@
         <v>27</v>
       </c>
       <c r="B111" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C111" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D111">
         <v>2015</v>
@@ -3230,13 +3230,13 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B112" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C112" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D112">
         <v>2015</v>
@@ -3256,10 +3256,10 @@
         <v>9</v>
       </c>
       <c r="B113" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C113" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D113">
         <v>2015</v>
@@ -3279,10 +3279,10 @@
         <v>7</v>
       </c>
       <c r="B114" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="C114" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D114">
         <v>2015</v>
@@ -3302,10 +3302,10 @@
         <v>19</v>
       </c>
       <c r="B115" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C115" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D115">
         <v>2015</v>
@@ -3325,10 +3325,10 @@
         <v>19</v>
       </c>
       <c r="B116" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C116" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D116">
         <v>2015</v>
@@ -3348,10 +3348,10 @@
         <v>13</v>
       </c>
       <c r="B117" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C117" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D117">
         <v>2015</v>
@@ -3371,10 +3371,10 @@
         <v>8</v>
       </c>
       <c r="B118" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="C118" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D118">
         <v>2015</v>
@@ -3394,10 +3394,10 @@
         <v>23</v>
       </c>
       <c r="B119" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C119" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="D119">
         <v>2015</v>
@@ -3417,10 +3417,10 @@
         <v>18</v>
       </c>
       <c r="B120" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C120" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D120">
         <v>2015</v>
@@ -3440,10 +3440,10 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C121" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D121">
         <v>2015</v>
@@ -3463,10 +3463,10 @@
         <v>10</v>
       </c>
       <c r="B122" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="C122" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D122">
         <v>2015</v>
@@ -3486,10 +3486,10 @@
         <v>3</v>
       </c>
       <c r="B123" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C123" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D123">
         <v>2015</v>
@@ -3509,10 +3509,10 @@
         <v>25</v>
       </c>
       <c r="B124" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C124" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D124">
         <v>2015</v>
@@ -3532,10 +3532,10 @@
         <v>12</v>
       </c>
       <c r="B125" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C125" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="D125">
         <v>2015</v>
@@ -3555,10 +3555,10 @@
         <v>5</v>
       </c>
       <c r="B126" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C126" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D126">
         <v>2015</v>
@@ -3578,10 +3578,10 @@
         <v>6</v>
       </c>
       <c r="B127" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="C127" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="D127">
         <v>2015</v>
@@ -3598,13 +3598,13 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B128" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C128" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D128">
         <v>2015</v>
@@ -3624,10 +3624,10 @@
         <v>20</v>
       </c>
       <c r="B129" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="C129" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D129">
         <v>2015</v>
@@ -3643,7 +3643,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E129">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G129">
     <sortCondition descending="1" ref="D1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>